<commit_message>
add mean and stdev
</commit_message>
<xml_diff>
--- a/Data_Gathering/Results_range.xlsx
+++ b/Data_Gathering/Results_range.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,11 +486,11 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45353</v>
+        <v>45356</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>02,03,04,17,35,36</t>
+          <t>03,18,24,35,40,41</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -531,11 +531,11 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45353</v>
+        <v>45356</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>02,03,04,17,35,36</t>
+          <t>03,18,24,35,40,41</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -576,11 +576,11 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45351</v>
+        <v>45353</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03,05,21,30,33,41</t>
+          <t>02,03,04,17,35,36</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -621,11 +621,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45351</v>
+        <v>45353</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>03,05,21,30,33,41</t>
+          <t>02,03,04,17,35,36</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -666,11 +666,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45349</v>
+        <v>45351</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26,31,32,39,40,41</t>
+          <t>03,05,21,30,33,41</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -711,11 +711,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45349</v>
+        <v>45351</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26,31,32,39,40,41</t>
+          <t>03,05,21,30,33,41</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -756,20 +756,110 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
+        <v>45349</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>26,31,32,39,40,41</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>day_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45349</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>26,31,32,39,40,41</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Within</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>month_day</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>34391</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>0,0,0,0,0,0</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>